<commit_message>
submitted draft nov 9
last working version as of nov 9, does not include changes from loopback...
</commit_message>
<xml_diff>
--- a/ballout_xl.xlsx
+++ b/ballout_xl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\GitHub\XL-manipulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarioIanniello\Documents\XL-manipulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F223B3F8-F71E-494E-BB5F-0CC98710D662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69369238-4B2C-4643-8FCE-608A144D3149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{33F5A552-C174-43E9-8A80-D353B920BD73}"/>
+    <workbookView xWindow="30" yWindow="450" windowWidth="28770" windowHeight="15750" xr2:uid="{955329A4-D43C-4798-82C1-B1938E53D2DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="170">
   <si>
     <t>A</t>
   </si>
@@ -257,7 +257,7 @@
     <t>TST_VDDQL_OPHY</t>
   </si>
   <si>
-    <t>TST_VSS</t>
+    <t>TST_VSS1</t>
   </si>
   <si>
     <t>DA6</t>
@@ -323,6 +323,9 @@
     <t>VDD18</t>
   </si>
   <si>
+    <t>TST_VSS2</t>
+  </si>
+  <si>
     <t>TST_VDDIO_OPHY</t>
   </si>
   <si>
@@ -380,6 +383,12 @@
     <t>AA</t>
   </si>
   <si>
+    <t>TST_VSS3</t>
+  </si>
+  <si>
+    <t>TST_VDDQ_OPHY</t>
+  </si>
+  <si>
     <t>VDDQ</t>
   </si>
   <si>
@@ -422,85 +431,31 @@
     <t>AF</t>
   </si>
   <si>
+    <t>DA37</t>
+  </si>
+  <si>
+    <t>DA35</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>VPP</t>
+  </si>
+  <si>
+    <t>DA36</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
     <t>VDDIO_TST</t>
   </si>
   <si>
-    <t>DA37</t>
-  </si>
-  <si>
-    <t>DA35</t>
-  </si>
-  <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ1</t>
-  </si>
-  <si>
-    <t>TST1_LB__RDQS_t</t>
-  </si>
-  <si>
-    <t>TST1_LB__RDQS_c</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ6</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ7</t>
-  </si>
-  <si>
-    <t>TST0_LB__WDQS_t</t>
-  </si>
-  <si>
-    <t>TST0_LB__WDQS_c</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ5</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ0</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ7</t>
-  </si>
-  <si>
-    <t>VPP</t>
-  </si>
-  <si>
-    <t>DA36</t>
-  </si>
-  <si>
-    <t>AH</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ3</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ5</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ0</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ2</t>
-  </si>
-  <si>
-    <t>TST1_LB__DQ4</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ2</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ4</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ6</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ1</t>
-  </si>
-  <si>
-    <t>TST0_LB__DQ3</t>
+    <t>VDDQL_TST</t>
+  </si>
+  <si>
+    <t>VDDQ_TST</t>
   </si>
   <si>
     <t>DA39</t>
@@ -512,9 +467,6 @@
     <t>AJ</t>
   </si>
   <si>
-    <t>VDDQL_TST</t>
-  </si>
-  <si>
     <t>TST3_GEN_IO_0</t>
   </si>
   <si>
@@ -543,9 +495,6 @@
   </si>
   <si>
     <t>TST2_DQ0</t>
-  </si>
-  <si>
-    <t>VDDQ_TST</t>
   </si>
   <si>
     <t>AK</t>
@@ -826,9 +775,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -838,10 +784,13 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pin" xfId="1" xr:uid="{84EEB76E-FC11-4CD6-A96C-91A6AEE4760A}"/>
+    <cellStyle name="Pin" xfId="1" xr:uid="{FF67FBE9-E5FC-4186-9BFF-E2E091E9FDFF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1152,11 +1101,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE00800B-FF06-4432-8DF3-206EA1E018AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95989C47-95D6-4E76-8C03-4CC8163CC065}">
   <dimension ref="B2:AF33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF32"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,20 +1605,20 @@
       <c r="H7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>1</v>
+      <c r="I7" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>1</v>
+      <c r="K7" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>1</v>
+      <c r="M7" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>31</v>
@@ -2616,10 +2565,10 @@
         <v>61</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>1</v>
@@ -2673,15 +2622,15 @@
         <v>1</v>
       </c>
       <c r="AE17" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF17" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1</v>
@@ -2769,15 +2718,15 @@
       </c>
       <c r="AE18" s="3"/>
       <c r="AF18" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>1</v>
@@ -2861,15 +2810,15 @@
         <v>1</v>
       </c>
       <c r="AE19" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AF19" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1</v>
@@ -2956,18 +2905,18 @@
         <v>19</v>
       </c>
       <c r="AE20" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AF20" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>1</v>
@@ -3054,12 +3003,12 @@
         <v>1</v>
       </c>
       <c r="AF21" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
@@ -3146,15 +3095,15 @@
         <v>19</v>
       </c>
       <c r="AE22" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AF22" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>61</v>
@@ -3190,34 +3139,34 @@
         <v>61</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Q23" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S23" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="T23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="U23" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="V23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="W23" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="X23" s="3" t="s">
         <v>1</v>
@@ -3244,12 +3193,12 @@
         <v>1</v>
       </c>
       <c r="AF23" s="11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>1</v>
@@ -3285,31 +3234,31 @@
         <v>1</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P24" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="R24" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="T24" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="V24" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="W24" s="3" t="s">
         <v>1</v>
@@ -3336,78 +3285,78 @@
         <v>19</v>
       </c>
       <c r="AE24" s="11" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AF24" s="11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O25" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O25" s="15" t="s">
-        <v>117</v>
-      </c>
       <c r="P25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="Q25" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="R25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S25" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="T25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="U25" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="V25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="W25" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="X25" s="3" t="s">
         <v>1</v>
@@ -3434,12 +3383,12 @@
         <v>1</v>
       </c>
       <c r="AF25" s="11" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>1</v>
@@ -3475,37 +3424,37 @@
         <v>1</v>
       </c>
       <c r="N26" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P26" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Q26" s="16" t="s">
         <v>1</v>
       </c>
       <c r="R26" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="S26" s="16" t="s">
         <v>1</v>
       </c>
       <c r="T26" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="U26" s="16" t="s">
         <v>1</v>
       </c>
       <c r="V26" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="W26" s="16" t="s">
         <v>1</v>
       </c>
       <c r="X26" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Y26" s="16" t="s">
         <v>1</v>
@@ -3526,15 +3475,15 @@
         <v>19</v>
       </c>
       <c r="AE26" s="18" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AF26" s="18" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>61</v>
@@ -3570,40 +3519,40 @@
         <v>61</v>
       </c>
       <c r="N27" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="O27" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="P27" s="16" t="s">
         <v>1</v>
       </c>
       <c r="Q27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="R27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="S27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="T27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="U27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="V27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="W27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="X27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Y27" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Z27" s="16" t="s">
         <v>1</v>
@@ -3624,39 +3573,39 @@
         <v>1</v>
       </c>
       <c r="AF27" s="18" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>1</v>
+        <v>130</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>1</v>
+      <c r="G28" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>1</v>
+      <c r="I28" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="J28" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>1</v>
+      <c r="K28" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="L28" s="12" t="s">
         <v>61</v>
@@ -3665,49 +3614,49 @@
         <v>1</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P28" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Q28" s="16" t="s">
         <v>1</v>
       </c>
       <c r="R28" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="S28" s="16" t="s">
         <v>1</v>
       </c>
       <c r="T28" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="U28" s="16" t="s">
         <v>1</v>
       </c>
       <c r="V28" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="W28" s="16" t="s">
         <v>1</v>
       </c>
       <c r="X28" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Y28" s="16" t="s">
         <v>1</v>
       </c>
       <c r="Z28" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA28" s="16" t="s">
         <v>1</v>
       </c>
       <c r="AB28" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AC28" s="3" t="s">
         <v>1</v>
@@ -3716,259 +3665,259 @@
         <v>19</v>
       </c>
       <c r="AE28" s="18" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AF28" s="18" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
-    <row r="29" spans="2:32" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="C29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="P29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="S29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="T29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="U29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="V29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="W29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="X29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="I29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J29" s="19" t="s">
+      <c r="AD29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF29" s="18" t="s">
         <v>135</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="L29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M29" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="N29" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="O29" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q29" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="R29" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="S29" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="T29" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="U29" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="V29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="W29" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="X29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC29" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF29" s="18" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="30" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K30" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="L30" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="M30" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="N30" s="19" t="s">
-        <v>151</v>
+      <c r="D30" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="J30" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L30" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="N30" s="16" t="s">
+        <v>1</v>
       </c>
       <c r="O30" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="P30" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q30" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="R30" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="S30" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="T30" s="16" t="s">
-        <v>1</v>
+      <c r="P30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="R30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="U30" s="16" t="s">
         <v>1</v>
       </c>
       <c r="V30" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="W30" s="16" t="s">
         <v>1</v>
       </c>
       <c r="X30" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Y30" s="16" t="s">
         <v>1</v>
       </c>
       <c r="Z30" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA30" s="16" t="s">
         <v>1</v>
       </c>
       <c r="AB30" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AC30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AD30" s="20" t="s">
-        <v>142</v>
+      <c r="AD30" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="AE30" s="18" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="AF30" s="18" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>158</v>
+        <v>142</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="F31" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G31" s="19" t="s">
-        <v>159</v>
+      <c r="G31" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I31" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="J31" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="L31" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="M31" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="N31" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="O31" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="P31" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q31" s="19" t="s">
-        <v>168</v>
+      <c r="I31" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="K31" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="L31" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="M31" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="N31" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="O31" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="P31" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q31" s="22" t="s">
+        <v>152</v>
       </c>
       <c r="R31" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="S31" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="T31" s="22" t="s">
-        <v>169</v>
+      <c r="S31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="T31" s="16" t="s">
+        <v>1</v>
       </c>
       <c r="U31" s="16" t="s">
         <v>1</v>
@@ -3986,22 +3935,22 @@
         <v>1</v>
       </c>
       <c r="Z31" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA31" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AB31" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="AC31" s="20" t="s">
-        <v>142</v>
+      <c r="AC31" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="AD31" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AE31" s="20" t="s">
-        <v>142</v>
+      <c r="AE31" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="AF31" s="3" t="s">
         <v>1</v>
@@ -4009,7 +3958,7 @@
     </row>
     <row r="32" spans="2:32" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>1</v>
@@ -4017,83 +3966,83 @@
       <c r="D32" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>172</v>
+      <c r="E32" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="19" t="s">
-        <v>173</v>
+      <c r="H32" s="22" t="s">
+        <v>156</v>
       </c>
       <c r="I32" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J32" s="19" t="s">
-        <v>174</v>
+      <c r="J32" s="22" t="s">
+        <v>157</v>
       </c>
       <c r="K32" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="L32" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="M32" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="N32" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="O32" s="19" t="s">
-        <v>178</v>
+      <c r="L32" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="M32" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="N32" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="O32" s="22" t="s">
+        <v>161</v>
       </c>
       <c r="P32" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="Q32" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="R32" s="19" t="s">
-        <v>180</v>
+      <c r="Q32" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="R32" s="22" t="s">
+        <v>163</v>
       </c>
       <c r="S32" s="16" t="s">
         <v>1</v>
       </c>
       <c r="T32" s="5" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="U32" s="5" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="V32" s="6" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="W32" s="5" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="X32" s="6" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="Y32" s="5" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="Z32" s="16" t="s">
         <v>1</v>
       </c>
       <c r="AA32" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AB32" s="14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AC32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AD32" s="20" t="s">
-        <v>142</v>
+      <c r="AD32" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="AE32" s="3" t="s">
         <v>1</v>

</xml_diff>